<commit_message>
New exercise classes. New Editor
</commit_message>
<xml_diff>
--- a/Files with Words/dictionary.xlsx
+++ b/Files with Words/dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikitazharinov/eclipse-workspace/wordflow_v3/Files with Words/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77D547B-131C-8A48-9038-866DFB855881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB64113-15B8-784E-8714-5BF5A68A72CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20500" activeTab="1" xr2:uid="{2E267A06-FA42-E34D-A83A-E5CE99E73D58}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6384" uniqueCount="3390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6381" uniqueCount="3390">
   <si>
     <t>ни . . . ни</t>
   </si>
@@ -32031,10 +32031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C15CFD-1121-2D45-9FF5-31F7FE805570}">
-  <dimension ref="A1:O488"/>
+  <dimension ref="A1:O487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A227" sqref="A227:XFD231"/>
+    <sheetView tabSelected="1" topLeftCell="A458" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B484" sqref="B484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35067,1760 +35067,1760 @@
       </c>
       <c r="E231" s="6"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A232" s="2" t="s">
+    <row r="232" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="6" t="s">
         <v>1291</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B232" s="6" t="s">
         <v>1290</v>
       </c>
-      <c r="C232" s="2"/>
-      <c r="D232" s="2" t="s">
+      <c r="C232" s="6"/>
+      <c r="D232" s="6" t="s">
         <v>1292</v>
       </c>
-      <c r="E232" s="2"/>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A233" s="2" t="s">
+      <c r="E232" s="6"/>
+    </row>
+    <row r="233" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="6" t="s">
         <v>1296</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B233" s="6" t="s">
         <v>1295</v>
       </c>
-      <c r="C233" s="2"/>
-      <c r="D233" s="2" t="s">
+      <c r="C233" s="6"/>
+      <c r="D233" s="6" t="s">
         <v>1297</v>
       </c>
-      <c r="E233" s="2"/>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A234" s="2" t="s">
+      <c r="E233" s="6"/>
+    </row>
+    <row r="234" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="6" t="s">
         <v>1301</v>
       </c>
-      <c r="B234" s="2" t="s">
+      <c r="B234" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="C234" s="2"/>
-      <c r="D234" s="2" t="s">
+      <c r="C234" s="6"/>
+      <c r="D234" s="6" t="s">
         <v>1302</v>
       </c>
-      <c r="E234" s="2"/>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A235" s="2" t="s">
+      <c r="E234" s="6"/>
+    </row>
+    <row r="235" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="6" t="s">
         <v>1306</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="B235" s="6" t="s">
         <v>1305</v>
       </c>
-      <c r="C235" s="2"/>
-      <c r="D235" s="2" t="s">
+      <c r="C235" s="6"/>
+      <c r="D235" s="6" t="s">
         <v>1307</v>
       </c>
-      <c r="E235" s="2"/>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A236" s="2" t="s">
+      <c r="E235" s="6"/>
+    </row>
+    <row r="236" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="6" t="s">
         <v>1311</v>
       </c>
-      <c r="B236" s="2" t="s">
+      <c r="B236" s="6" t="s">
         <v>1310</v>
       </c>
-      <c r="C236" s="2"/>
-      <c r="D236" s="2" t="s">
+      <c r="C236" s="6"/>
+      <c r="D236" s="6" t="s">
         <v>1312</v>
       </c>
-      <c r="E236" s="2"/>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A237" s="2" t="s">
+      <c r="E236" s="6"/>
+    </row>
+    <row r="237" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="6" t="s">
         <v>1316</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="B237" s="6" t="s">
         <v>1315</v>
       </c>
-      <c r="C237" s="2"/>
-      <c r="D237" s="2" t="s">
+      <c r="C237" s="6"/>
+      <c r="D237" s="6" t="s">
         <v>1317</v>
       </c>
-      <c r="E237" s="2"/>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A238" s="2" t="s">
+      <c r="E237" s="6"/>
+    </row>
+    <row r="238" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="6" t="s">
         <v>1321</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="B238" s="6" t="s">
         <v>1320</v>
       </c>
-      <c r="C238" s="2"/>
-      <c r="D238" s="2" t="s">
+      <c r="C238" s="6"/>
+      <c r="D238" s="6" t="s">
         <v>1322</v>
       </c>
-      <c r="E238" s="2"/>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A239" s="2" t="s">
+      <c r="E238" s="6"/>
+    </row>
+    <row r="239" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="6" t="s">
         <v>1326</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" s="6" t="s">
         <v>1325</v>
       </c>
-      <c r="C239" s="2"/>
-      <c r="D239" s="2" t="s">
+      <c r="C239" s="6"/>
+      <c r="D239" s="6" t="s">
         <v>1327</v>
       </c>
-      <c r="E239" s="2"/>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A240" s="2" t="s">
+      <c r="E239" s="6"/>
+    </row>
+    <row r="240" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="6" t="s">
         <v>1331</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="B240" s="6" t="s">
         <v>1330</v>
       </c>
-      <c r="C240" s="2"/>
-      <c r="D240" s="2" t="s">
+      <c r="C240" s="6"/>
+      <c r="D240" s="6" t="s">
         <v>1332</v>
       </c>
-      <c r="E240" s="2"/>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A241" s="2" t="s">
+      <c r="E240" s="6"/>
+    </row>
+    <row r="241" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="6" t="s">
         <v>1336</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B241" s="6" t="s">
         <v>1335</v>
       </c>
-      <c r="C241" s="2"/>
-      <c r="D241" s="2" t="s">
+      <c r="C241" s="6"/>
+      <c r="D241" s="6" t="s">
         <v>1337</v>
       </c>
-      <c r="E241" s="2"/>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A242" s="2" t="s">
+      <c r="E241" s="6"/>
+    </row>
+    <row r="242" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="6" t="s">
         <v>1341</v>
       </c>
-      <c r="B242" s="2" t="s">
+      <c r="B242" s="6" t="s">
         <v>1340</v>
       </c>
-      <c r="C242" s="2"/>
-      <c r="D242" s="2" t="s">
+      <c r="C242" s="6"/>
+      <c r="D242" s="6" t="s">
         <v>1342</v>
       </c>
-      <c r="E242" s="2"/>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A243" s="2" t="s">
+      <c r="E242" s="6"/>
+    </row>
+    <row r="243" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="6" t="s">
         <v>1346</v>
       </c>
-      <c r="B243" s="2" t="s">
+      <c r="B243" s="6" t="s">
         <v>1345</v>
       </c>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2" t="s">
+      <c r="C243" s="6"/>
+      <c r="D243" s="6" t="s">
         <v>1347</v>
       </c>
-      <c r="E243" s="2"/>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A244" s="2" t="s">
+      <c r="E243" s="6"/>
+    </row>
+    <row r="244" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="6" t="s">
         <v>1351</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B244" s="6" t="s">
         <v>1350</v>
       </c>
-      <c r="C244" s="2"/>
-      <c r="D244" s="2" t="s">
+      <c r="C244" s="6"/>
+      <c r="D244" s="6" t="s">
         <v>1352</v>
       </c>
-      <c r="E244" s="2"/>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A245" s="2" t="s">
+      <c r="E244" s="6"/>
+    </row>
+    <row r="245" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="6" t="s">
         <v>1356</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="B245" s="6" t="s">
         <v>1355</v>
       </c>
-      <c r="C245" s="2"/>
-      <c r="D245" s="2" t="s">
+      <c r="C245" s="6"/>
+      <c r="D245" s="6" t="s">
         <v>1357</v>
       </c>
-      <c r="E245" s="2"/>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A246" s="2" t="s">
+      <c r="E245" s="6"/>
+    </row>
+    <row r="246" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="6" t="s">
         <v>1361</v>
       </c>
-      <c r="B246" s="2" t="s">
+      <c r="B246" s="6" t="s">
         <v>1360</v>
       </c>
-      <c r="C246" s="2"/>
-      <c r="D246" s="2" t="s">
+      <c r="C246" s="6"/>
+      <c r="D246" s="6" t="s">
         <v>1362</v>
       </c>
-      <c r="E246" s="2"/>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A247" s="2" t="s">
+      <c r="E246" s="6"/>
+    </row>
+    <row r="247" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="6" t="s">
         <v>1366</v>
       </c>
-      <c r="B247" s="2" t="s">
+      <c r="B247" s="6" t="s">
         <v>1365</v>
       </c>
-      <c r="C247" s="2"/>
-      <c r="D247" s="2" t="s">
+      <c r="C247" s="6"/>
+      <c r="D247" s="6" t="s">
         <v>1367</v>
       </c>
-      <c r="E247" s="2"/>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A248" s="2" t="s">
+      <c r="E247" s="6"/>
+    </row>
+    <row r="248" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="6" t="s">
         <v>1371</v>
       </c>
-      <c r="B248" s="2" t="s">
+      <c r="B248" s="6" t="s">
         <v>1370</v>
       </c>
-      <c r="C248" s="2"/>
-      <c r="D248" s="2" t="s">
+      <c r="C248" s="6"/>
+      <c r="D248" s="6" t="s">
         <v>1372</v>
       </c>
-      <c r="E248" s="2"/>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A249" s="2" t="s">
+      <c r="E248" s="6"/>
+    </row>
+    <row r="249" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="6" t="s">
         <v>1376</v>
       </c>
-      <c r="B249" s="2" t="s">
+      <c r="B249" s="6" t="s">
         <v>1375</v>
       </c>
-      <c r="C249" s="2"/>
-      <c r="D249" s="2" t="s">
+      <c r="C249" s="6"/>
+      <c r="D249" s="6" t="s">
         <v>1377</v>
       </c>
-      <c r="E249" s="2"/>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A250" s="2" t="s">
+      <c r="E249" s="6"/>
+    </row>
+    <row r="250" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="6" t="s">
         <v>1381</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="B250" s="6" t="s">
         <v>1380</v>
       </c>
-      <c r="C250" s="2"/>
-      <c r="D250" s="2" t="s">
+      <c r="C250" s="6"/>
+      <c r="D250" s="6" t="s">
         <v>1382</v>
       </c>
-      <c r="E250" s="2"/>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A251" s="2" t="s">
+      <c r="E250" s="6"/>
+    </row>
+    <row r="251" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="6" t="s">
         <v>1386</v>
       </c>
-      <c r="B251" s="2" t="s">
+      <c r="B251" s="6" t="s">
         <v>1385</v>
       </c>
-      <c r="C251" s="2"/>
-      <c r="D251" s="2" t="s">
+      <c r="C251" s="6"/>
+      <c r="D251" s="6" t="s">
         <v>1387</v>
       </c>
-      <c r="E251" s="2"/>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A252" s="2" t="s">
+      <c r="E251" s="6"/>
+    </row>
+    <row r="252" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="6" t="s">
         <v>1391</v>
       </c>
-      <c r="B252" s="2" t="s">
+      <c r="B252" s="6" t="s">
         <v>1390</v>
       </c>
-      <c r="C252" s="2"/>
-      <c r="D252" s="2" t="s">
+      <c r="C252" s="6"/>
+      <c r="D252" s="6" t="s">
         <v>1392</v>
       </c>
-      <c r="E252" s="2"/>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A253" s="2" t="s">
+      <c r="E252" s="6"/>
+    </row>
+    <row r="253" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="6" t="s">
         <v>1396</v>
       </c>
-      <c r="B253" s="2" t="s">
+      <c r="B253" s="6" t="s">
         <v>1395</v>
       </c>
-      <c r="C253" s="2"/>
-      <c r="D253" s="2" t="s">
+      <c r="C253" s="6"/>
+      <c r="D253" s="6" t="s">
         <v>1397</v>
       </c>
-      <c r="E253" s="2"/>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A254" s="2" t="s">
+      <c r="E253" s="6"/>
+    </row>
+    <row r="254" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="6" t="s">
         <v>1401</v>
       </c>
-      <c r="B254" s="2" t="s">
+      <c r="B254" s="6" t="s">
         <v>1400</v>
       </c>
-      <c r="C254" s="2"/>
-      <c r="D254" s="2" t="s">
+      <c r="C254" s="6"/>
+      <c r="D254" s="6" t="s">
         <v>1402</v>
       </c>
-      <c r="E254" s="2"/>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A255" s="2" t="s">
+      <c r="E254" s="6"/>
+    </row>
+    <row r="255" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="6" t="s">
         <v>1406</v>
       </c>
-      <c r="B255" s="2" t="s">
+      <c r="B255" s="6" t="s">
         <v>1405</v>
       </c>
-      <c r="C255" s="2"/>
-      <c r="D255" s="2" t="s">
+      <c r="C255" s="6"/>
+      <c r="D255" s="6" t="s">
         <v>1407</v>
       </c>
-      <c r="E255" s="2"/>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A256" s="2" t="s">
+      <c r="E255" s="6"/>
+    </row>
+    <row r="256" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="6" t="s">
         <v>1411</v>
       </c>
-      <c r="B256" s="2" t="s">
+      <c r="B256" s="6" t="s">
         <v>1410</v>
       </c>
-      <c r="C256" s="2"/>
-      <c r="D256" s="2" t="s">
+      <c r="C256" s="6"/>
+      <c r="D256" s="6" t="s">
         <v>1412</v>
       </c>
-      <c r="E256" s="2"/>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A257" s="2" t="s">
+      <c r="E256" s="6"/>
+    </row>
+    <row r="257" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="6" t="s">
         <v>1416</v>
       </c>
-      <c r="B257" s="2" t="s">
+      <c r="B257" s="6" t="s">
         <v>1415</v>
       </c>
-      <c r="C257" s="2"/>
-      <c r="D257" s="2" t="s">
+      <c r="C257" s="6"/>
+      <c r="D257" s="6" t="s">
         <v>1417</v>
       </c>
-      <c r="E257" s="2"/>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A258" s="2" t="s">
+      <c r="E257" s="6"/>
+    </row>
+    <row r="258" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="6" t="s">
         <v>1421</v>
       </c>
-      <c r="B258" s="2" t="s">
+      <c r="B258" s="6" t="s">
         <v>1420</v>
       </c>
-      <c r="C258" s="2"/>
-      <c r="D258" s="2" t="s">
+      <c r="C258" s="6"/>
+      <c r="D258" s="6" t="s">
         <v>1422</v>
       </c>
-      <c r="E258" s="2"/>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A259" s="2" t="s">
+      <c r="E258" s="6"/>
+    </row>
+    <row r="259" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="6" t="s">
         <v>1426</v>
       </c>
-      <c r="B259" s="2" t="s">
+      <c r="B259" s="6" t="s">
         <v>1425</v>
       </c>
-      <c r="C259" s="2"/>
-      <c r="D259" s="2" t="s">
+      <c r="C259" s="6"/>
+      <c r="D259" s="6" t="s">
         <v>1427</v>
       </c>
-      <c r="E259" s="2"/>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A260" s="2" t="s">
+      <c r="E259" s="6"/>
+    </row>
+    <row r="260" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="6" t="s">
         <v>1431</v>
       </c>
-      <c r="B260" s="2" t="s">
+      <c r="B260" s="6" t="s">
         <v>1430</v>
       </c>
-      <c r="C260" s="2"/>
-      <c r="D260" s="2" t="s">
+      <c r="C260" s="6"/>
+      <c r="D260" s="6" t="s">
         <v>1432</v>
       </c>
-      <c r="E260" s="2"/>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A261" s="2" t="s">
+      <c r="E260" s="6"/>
+    </row>
+    <row r="261" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="6" t="s">
         <v>1436</v>
       </c>
-      <c r="B261" s="2" t="s">
+      <c r="B261" s="6" t="s">
         <v>1435</v>
       </c>
-      <c r="C261" s="2"/>
-      <c r="D261" s="2" t="s">
+      <c r="C261" s="6"/>
+      <c r="D261" s="6" t="s">
         <v>1437</v>
       </c>
-      <c r="E261" s="2"/>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A262" s="2" t="s">
+      <c r="E261" s="6"/>
+    </row>
+    <row r="262" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="6" t="s">
         <v>1441</v>
       </c>
-      <c r="B262" s="2" t="s">
+      <c r="B262" s="6" t="s">
         <v>1440</v>
       </c>
-      <c r="C262" s="2"/>
-      <c r="D262" s="2" t="s">
+      <c r="C262" s="6"/>
+      <c r="D262" s="6" t="s">
         <v>1442</v>
       </c>
-      <c r="E262" s="2"/>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A263" s="2" t="s">
+      <c r="E262" s="6"/>
+    </row>
+    <row r="263" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="6" t="s">
         <v>1446</v>
       </c>
-      <c r="B263" s="2" t="s">
+      <c r="B263" s="6" t="s">
         <v>1445</v>
       </c>
-      <c r="C263" s="2"/>
-      <c r="D263" s="2" t="s">
+      <c r="C263" s="6"/>
+      <c r="D263" s="6" t="s">
         <v>1447</v>
       </c>
-      <c r="E263" s="2"/>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A264" s="2" t="s">
+      <c r="E263" s="6"/>
+    </row>
+    <row r="264" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A264" s="6" t="s">
         <v>1451</v>
       </c>
-      <c r="B264" s="2" t="s">
+      <c r="B264" s="6" t="s">
         <v>1450</v>
       </c>
-      <c r="C264" s="2"/>
-      <c r="D264" s="2" t="s">
+      <c r="C264" s="6"/>
+      <c r="D264" s="6" t="s">
         <v>1452</v>
       </c>
-      <c r="E264" s="2"/>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A265" s="2" t="s">
+      <c r="E264" s="6"/>
+    </row>
+    <row r="265" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="6" t="s">
         <v>1456</v>
       </c>
-      <c r="B265" s="2" t="s">
+      <c r="B265" s="6" t="s">
         <v>1455</v>
       </c>
-      <c r="C265" s="2"/>
-      <c r="D265" s="2" t="s">
+      <c r="C265" s="6"/>
+      <c r="D265" s="6" t="s">
         <v>1457</v>
       </c>
-      <c r="E265" s="2"/>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A266" s="2" t="s">
+      <c r="E265" s="6"/>
+    </row>
+    <row r="266" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="6" t="s">
         <v>1461</v>
       </c>
-      <c r="B266" s="2" t="s">
+      <c r="B266" s="6" t="s">
         <v>1460</v>
       </c>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2" t="s">
+      <c r="C266" s="6"/>
+      <c r="D266" s="6" t="s">
         <v>1462</v>
       </c>
-      <c r="E266" s="2"/>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A267" s="2" t="s">
+      <c r="E266" s="6"/>
+    </row>
+    <row r="267" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A267" s="6" t="s">
         <v>1466</v>
       </c>
-      <c r="B267" s="2" t="s">
+      <c r="B267" s="6" t="s">
         <v>1465</v>
       </c>
-      <c r="C267" s="2"/>
-      <c r="D267" s="2" t="s">
+      <c r="C267" s="6"/>
+      <c r="D267" s="6" t="s">
         <v>1467</v>
       </c>
-      <c r="E267" s="2"/>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A268" s="2" t="s">
+      <c r="E267" s="6"/>
+    </row>
+    <row r="268" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A268" s="6" t="s">
         <v>1471</v>
       </c>
-      <c r="B268" s="2" t="s">
+      <c r="B268" s="6" t="s">
         <v>1470</v>
       </c>
-      <c r="C268" s="2"/>
-      <c r="D268" s="2" t="s">
+      <c r="C268" s="6"/>
+      <c r="D268" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="E268" s="2"/>
-    </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A269" s="2" t="s">
+      <c r="E268" s="6"/>
+    </row>
+    <row r="269" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A269" s="6" t="s">
         <v>1476</v>
       </c>
-      <c r="B269" s="2" t="s">
+      <c r="B269" s="6" t="s">
         <v>1475</v>
       </c>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2" t="s">
+      <c r="C269" s="6"/>
+      <c r="D269" s="6" t="s">
         <v>1477</v>
       </c>
-      <c r="E269" s="2"/>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A270" s="2" t="s">
+      <c r="E269" s="6"/>
+    </row>
+    <row r="270" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A270" s="6" t="s">
         <v>1481</v>
       </c>
-      <c r="B270" s="2" t="s">
+      <c r="B270" s="6" t="s">
         <v>1480</v>
       </c>
-      <c r="C270" s="2"/>
-      <c r="D270" s="2" t="s">
+      <c r="C270" s="6"/>
+      <c r="D270" s="6" t="s">
         <v>1482</v>
       </c>
-      <c r="E270" s="2"/>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A271" s="2" t="s">
+      <c r="E270" s="6"/>
+    </row>
+    <row r="271" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="6" t="s">
         <v>1486</v>
       </c>
-      <c r="B271" s="2" t="s">
+      <c r="B271" s="6" t="s">
         <v>1485</v>
       </c>
-      <c r="C271" s="2"/>
-      <c r="D271" s="2" t="s">
+      <c r="C271" s="6"/>
+      <c r="D271" s="6" t="s">
         <v>1487</v>
       </c>
-      <c r="E271" s="2"/>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A272" s="2" t="s">
+      <c r="E271" s="6"/>
+    </row>
+    <row r="272" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="6" t="s">
         <v>1491</v>
       </c>
-      <c r="B272" s="2" t="s">
+      <c r="B272" s="6" t="s">
         <v>1490</v>
       </c>
-      <c r="C272" s="2"/>
-      <c r="D272" s="2" t="s">
+      <c r="C272" s="6"/>
+      <c r="D272" s="6" t="s">
         <v>1492</v>
       </c>
-      <c r="E272" s="2"/>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A273" s="2" t="s">
+      <c r="E272" s="6"/>
+    </row>
+    <row r="273" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A273" s="6" t="s">
         <v>1496</v>
       </c>
-      <c r="B273" s="2" t="s">
+      <c r="B273" s="6" t="s">
         <v>1495</v>
       </c>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2" t="s">
+      <c r="C273" s="6"/>
+      <c r="D273" s="6" t="s">
         <v>1497</v>
       </c>
-      <c r="E273" s="2"/>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A274" s="2" t="s">
+      <c r="E273" s="6"/>
+    </row>
+    <row r="274" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A274" s="6" t="s">
         <v>1501</v>
       </c>
-      <c r="B274" s="2" t="s">
+      <c r="B274" s="6" t="s">
         <v>1500</v>
       </c>
-      <c r="C274" s="2"/>
-      <c r="D274" s="2" t="s">
+      <c r="C274" s="6"/>
+      <c r="D274" s="6" t="s">
         <v>1502</v>
       </c>
-      <c r="E274" s="2"/>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A275" s="2" t="s">
+      <c r="E274" s="6"/>
+    </row>
+    <row r="275" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="6" t="s">
         <v>1506</v>
       </c>
-      <c r="B275" s="2" t="s">
+      <c r="B275" s="6" t="s">
         <v>1505</v>
       </c>
-      <c r="C275" s="2"/>
-      <c r="D275" s="2" t="s">
+      <c r="C275" s="6"/>
+      <c r="D275" s="6" t="s">
         <v>1507</v>
       </c>
-      <c r="E275" s="2"/>
-    </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A276" s="2" t="s">
+      <c r="E275" s="6"/>
+    </row>
+    <row r="276" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="6" t="s">
         <v>1511</v>
       </c>
-      <c r="B276" s="2" t="s">
+      <c r="B276" s="6" t="s">
         <v>1510</v>
       </c>
-      <c r="C276" s="2"/>
-      <c r="D276" s="2" t="s">
+      <c r="C276" s="6"/>
+      <c r="D276" s="6" t="s">
         <v>1512</v>
       </c>
-      <c r="E276" s="2"/>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A277" s="2" t="s">
+      <c r="E276" s="6"/>
+    </row>
+    <row r="277" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="6" t="s">
         <v>1516</v>
       </c>
-      <c r="B277" s="2" t="s">
+      <c r="B277" s="6" t="s">
         <v>1515</v>
       </c>
-      <c r="C277" s="2"/>
-      <c r="D277" s="2" t="s">
+      <c r="C277" s="6"/>
+      <c r="D277" s="6" t="s">
         <v>1517</v>
       </c>
-      <c r="E277" s="2"/>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A278" s="2" t="s">
+      <c r="E277" s="6"/>
+    </row>
+    <row r="278" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="6" t="s">
         <v>1521</v>
       </c>
-      <c r="B278" s="2" t="s">
+      <c r="B278" s="6" t="s">
         <v>1520</v>
       </c>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2" t="s">
+      <c r="C278" s="6"/>
+      <c r="D278" s="6" t="s">
         <v>1522</v>
       </c>
-      <c r="E278" s="2"/>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A279" s="2" t="s">
+      <c r="E278" s="6"/>
+    </row>
+    <row r="279" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="6" t="s">
         <v>1526</v>
       </c>
-      <c r="B279" s="2" t="s">
+      <c r="B279" s="6" t="s">
         <v>1525</v>
       </c>
-      <c r="C279" s="2"/>
-      <c r="D279" s="2" t="s">
+      <c r="C279" s="6"/>
+      <c r="D279" s="6" t="s">
         <v>1527</v>
       </c>
-      <c r="E279" s="2"/>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A280" s="2" t="s">
+      <c r="E279" s="6"/>
+    </row>
+    <row r="280" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="6" t="s">
         <v>1531</v>
       </c>
-      <c r="B280" s="2" t="s">
+      <c r="B280" s="6" t="s">
         <v>1530</v>
       </c>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2" t="s">
+      <c r="C280" s="6"/>
+      <c r="D280" s="6" t="s">
         <v>1532</v>
       </c>
-      <c r="E280" s="2"/>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A281" s="2" t="s">
+      <c r="E280" s="6"/>
+    </row>
+    <row r="281" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="6" t="s">
         <v>1536</v>
       </c>
-      <c r="B281" s="2" t="s">
+      <c r="B281" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2" t="s">
+      <c r="C281" s="6"/>
+      <c r="D281" s="6" t="s">
         <v>1537</v>
       </c>
-      <c r="E281" s="2"/>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A282" s="2" t="s">
+      <c r="E281" s="6"/>
+    </row>
+    <row r="282" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="6" t="s">
         <v>1541</v>
       </c>
-      <c r="B282" s="2" t="s">
+      <c r="B282" s="6" t="s">
         <v>1540</v>
       </c>
-      <c r="C282" s="2"/>
-      <c r="D282" s="2" t="s">
+      <c r="C282" s="6"/>
+      <c r="D282" s="6" t="s">
         <v>1542</v>
       </c>
-      <c r="E282" s="2"/>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A283" s="2" t="s">
+      <c r="E282" s="6"/>
+    </row>
+    <row r="283" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="6" t="s">
         <v>1546</v>
       </c>
-      <c r="B283" s="2" t="s">
+      <c r="B283" s="6" t="s">
         <v>1545</v>
       </c>
-      <c r="C283" s="2"/>
-      <c r="D283" s="2" t="s">
+      <c r="C283" s="6"/>
+      <c r="D283" s="6" t="s">
         <v>1547</v>
       </c>
-      <c r="E283" s="2"/>
-    </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A284" s="2" t="s">
+      <c r="E283" s="6"/>
+    </row>
+    <row r="284" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="6" t="s">
         <v>1551</v>
       </c>
-      <c r="B284" s="2" t="s">
+      <c r="B284" s="6" t="s">
         <v>1550</v>
       </c>
-      <c r="C284" s="2"/>
-      <c r="D284" s="2" t="s">
+      <c r="C284" s="6"/>
+      <c r="D284" s="6" t="s">
         <v>1552</v>
       </c>
-      <c r="E284" s="2"/>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A285" s="2" t="s">
+      <c r="E284" s="6"/>
+    </row>
+    <row r="285" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="6" t="s">
         <v>1556</v>
       </c>
-      <c r="B285" s="2" t="s">
+      <c r="B285" s="6" t="s">
         <v>1555</v>
       </c>
-      <c r="C285" s="2"/>
-      <c r="D285" s="2" t="s">
+      <c r="C285" s="6"/>
+      <c r="D285" s="6" t="s">
         <v>1557</v>
       </c>
-      <c r="E285" s="2"/>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A286" s="2" t="s">
+      <c r="E285" s="6"/>
+    </row>
+    <row r="286" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="6" t="s">
         <v>1561</v>
       </c>
-      <c r="B286" s="2" t="s">
+      <c r="B286" s="6" t="s">
         <v>1560</v>
       </c>
-      <c r="C286" s="2"/>
-      <c r="D286" s="2" t="s">
+      <c r="C286" s="6"/>
+      <c r="D286" s="6" t="s">
         <v>1562</v>
       </c>
-      <c r="E286" s="2"/>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" s="2" t="s">
+      <c r="E286" s="6"/>
+    </row>
+    <row r="287" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A287" s="6" t="s">
         <v>1566</v>
       </c>
-      <c r="B287" s="2" t="s">
+      <c r="B287" s="6" t="s">
         <v>1565</v>
       </c>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2" t="s">
+      <c r="C287" s="6"/>
+      <c r="D287" s="6" t="s">
         <v>1567</v>
       </c>
-      <c r="E287" s="2"/>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" s="2" t="s">
+      <c r="E287" s="6"/>
+    </row>
+    <row r="288" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A288" s="6" t="s">
         <v>1571</v>
       </c>
-      <c r="B288" s="2" t="s">
+      <c r="B288" s="6" t="s">
         <v>1570</v>
       </c>
-      <c r="C288" s="2"/>
-      <c r="D288" s="2" t="s">
+      <c r="C288" s="6"/>
+      <c r="D288" s="6" t="s">
         <v>1572</v>
       </c>
-      <c r="E288" s="2"/>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" s="2" t="s">
+      <c r="E288" s="6"/>
+    </row>
+    <row r="289" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="6" t="s">
         <v>1576</v>
       </c>
-      <c r="B289" s="2" t="s">
+      <c r="B289" s="6" t="s">
         <v>1575</v>
       </c>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2" t="s">
+      <c r="C289" s="6"/>
+      <c r="D289" s="6" t="s">
         <v>1577</v>
       </c>
-      <c r="E289" s="2"/>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A290" s="2" t="s">
+      <c r="E289" s="6"/>
+    </row>
+    <row r="290" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="6" t="s">
         <v>1581</v>
       </c>
-      <c r="B290" s="2" t="s">
+      <c r="B290" s="6" t="s">
         <v>1580</v>
       </c>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2" t="s">
+      <c r="C290" s="6"/>
+      <c r="D290" s="6" t="s">
         <v>1582</v>
       </c>
-      <c r="E290" s="2"/>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A291" s="2" t="s">
+      <c r="E290" s="6"/>
+    </row>
+    <row r="291" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="6" t="s">
         <v>1586</v>
       </c>
-      <c r="B291" s="2" t="s">
+      <c r="B291" s="6" t="s">
         <v>1585</v>
       </c>
-      <c r="C291" s="2"/>
-      <c r="D291" s="2" t="s">
+      <c r="C291" s="6"/>
+      <c r="D291" s="6" t="s">
         <v>1587</v>
       </c>
-      <c r="E291" s="2"/>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" s="2" t="s">
+      <c r="E291" s="6"/>
+    </row>
+    <row r="292" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="6" t="s">
         <v>1591</v>
       </c>
-      <c r="B292" s="2" t="s">
+      <c r="B292" s="6" t="s">
         <v>1590</v>
       </c>
-      <c r="C292" s="2"/>
-      <c r="D292" s="2" t="s">
+      <c r="C292" s="6"/>
+      <c r="D292" s="6" t="s">
         <v>1592</v>
       </c>
-      <c r="E292" s="2"/>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A293" s="2" t="s">
+      <c r="E292" s="6"/>
+    </row>
+    <row r="293" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A293" s="6" t="s">
         <v>1596</v>
       </c>
-      <c r="B293" s="2" t="s">
+      <c r="B293" s="6" t="s">
         <v>1595</v>
       </c>
-      <c r="C293" s="2"/>
-      <c r="D293" s="2" t="s">
+      <c r="C293" s="6"/>
+      <c r="D293" s="6" t="s">
         <v>1597</v>
       </c>
-      <c r="E293" s="2"/>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A294" s="2" t="s">
+      <c r="E293" s="6"/>
+    </row>
+    <row r="294" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A294" s="6" t="s">
         <v>1601</v>
       </c>
-      <c r="B294" s="2" t="s">
+      <c r="B294" s="6" t="s">
         <v>1600</v>
       </c>
-      <c r="C294" s="2"/>
-      <c r="D294" s="2" t="s">
+      <c r="C294" s="6"/>
+      <c r="D294" s="6" t="s">
         <v>1602</v>
       </c>
-      <c r="E294" s="2"/>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A295" s="2" t="s">
+      <c r="E294" s="6"/>
+    </row>
+    <row r="295" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="6" t="s">
         <v>1606</v>
       </c>
-      <c r="B295" s="2" t="s">
+      <c r="B295" s="6" t="s">
         <v>1605</v>
       </c>
-      <c r="C295" s="2"/>
-      <c r="D295" s="2" t="s">
+      <c r="C295" s="6"/>
+      <c r="D295" s="6" t="s">
         <v>1607</v>
       </c>
-      <c r="E295" s="2"/>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A296" s="2" t="s">
+      <c r="E295" s="6"/>
+    </row>
+    <row r="296" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A296" s="6" t="s">
         <v>1611</v>
       </c>
-      <c r="B296" s="2" t="s">
+      <c r="B296" s="6" t="s">
         <v>1610</v>
       </c>
-      <c r="C296" s="2"/>
-      <c r="D296" s="2" t="s">
+      <c r="C296" s="6"/>
+      <c r="D296" s="6" t="s">
         <v>1612</v>
       </c>
-      <c r="E296" s="2"/>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A297" s="2" t="s">
+      <c r="E296" s="6"/>
+    </row>
+    <row r="297" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A297" s="6" t="s">
         <v>1616</v>
       </c>
-      <c r="B297" s="2" t="s">
+      <c r="B297" s="6" t="s">
         <v>1615</v>
       </c>
-      <c r="C297" s="2"/>
-      <c r="D297" s="2" t="s">
+      <c r="C297" s="6"/>
+      <c r="D297" s="6" t="s">
         <v>1617</v>
       </c>
-      <c r="E297" s="2"/>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" s="2" t="s">
+      <c r="E297" s="6"/>
+    </row>
+    <row r="298" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="6" t="s">
         <v>1621</v>
       </c>
-      <c r="B298" s="2" t="s">
+      <c r="B298" s="6" t="s">
         <v>1620</v>
       </c>
-      <c r="C298" s="2"/>
-      <c r="D298" s="2" t="s">
+      <c r="C298" s="6"/>
+      <c r="D298" s="6" t="s">
         <v>1622</v>
       </c>
-      <c r="E298" s="2"/>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A299" s="2" t="s">
+      <c r="E298" s="6"/>
+    </row>
+    <row r="299" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="6" t="s">
         <v>1626</v>
       </c>
-      <c r="B299" s="2" t="s">
+      <c r="B299" s="6" t="s">
         <v>1625</v>
       </c>
-      <c r="C299" s="2"/>
-      <c r="D299" s="2" t="s">
+      <c r="C299" s="6"/>
+      <c r="D299" s="6" t="s">
         <v>1627</v>
       </c>
-      <c r="E299" s="2"/>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" s="2" t="s">
+      <c r="E299" s="6"/>
+    </row>
+    <row r="300" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A300" s="6" t="s">
         <v>1631</v>
       </c>
-      <c r="B300" s="2" t="s">
+      <c r="B300" s="6" t="s">
         <v>1630</v>
       </c>
-      <c r="C300" s="2"/>
-      <c r="D300" s="2" t="s">
+      <c r="C300" s="6"/>
+      <c r="D300" s="6" t="s">
         <v>1632</v>
       </c>
-      <c r="E300" s="2"/>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A301" s="2" t="s">
+      <c r="E300" s="6"/>
+    </row>
+    <row r="301" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A301" s="6" t="s">
         <v>1636</v>
       </c>
-      <c r="B301" s="2" t="s">
+      <c r="B301" s="6" t="s">
         <v>1635</v>
       </c>
-      <c r="C301" s="2"/>
-      <c r="D301" s="2" t="s">
+      <c r="C301" s="6"/>
+      <c r="D301" s="6" t="s">
         <v>1637</v>
       </c>
-      <c r="E301" s="2"/>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" s="2" t="s">
+      <c r="E301" s="6"/>
+    </row>
+    <row r="302" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A302" s="6" t="s">
         <v>1641</v>
       </c>
-      <c r="B302" s="2" t="s">
+      <c r="B302" s="6" t="s">
         <v>1640</v>
       </c>
-      <c r="C302" s="2"/>
-      <c r="D302" s="2" t="s">
+      <c r="C302" s="6"/>
+      <c r="D302" s="6" t="s">
         <v>1642</v>
       </c>
-      <c r="E302" s="2"/>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A303" s="2" t="s">
+      <c r="E302" s="6"/>
+    </row>
+    <row r="303" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="6" t="s">
         <v>1646</v>
       </c>
-      <c r="B303" s="2" t="s">
+      <c r="B303" s="6" t="s">
         <v>1645</v>
       </c>
-      <c r="C303" s="2"/>
-      <c r="D303" s="2" t="s">
+      <c r="C303" s="6"/>
+      <c r="D303" s="6" t="s">
         <v>1647</v>
       </c>
-      <c r="E303" s="2"/>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" s="2" t="s">
+      <c r="E303" s="6"/>
+    </row>
+    <row r="304" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="6" t="s">
         <v>1651</v>
       </c>
-      <c r="B304" s="2" t="s">
+      <c r="B304" s="6" t="s">
         <v>1650</v>
       </c>
-      <c r="C304" s="2"/>
-      <c r="D304" s="2" t="s">
+      <c r="C304" s="6"/>
+      <c r="D304" s="6" t="s">
         <v>1652</v>
       </c>
-      <c r="E304" s="2"/>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A305" s="2" t="s">
+      <c r="E304" s="6"/>
+    </row>
+    <row r="305" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="6" t="s">
         <v>1656</v>
       </c>
-      <c r="B305" s="2" t="s">
+      <c r="B305" s="6" t="s">
         <v>1655</v>
       </c>
-      <c r="C305" s="2"/>
-      <c r="D305" s="2" t="s">
+      <c r="C305" s="6"/>
+      <c r="D305" s="6" t="s">
         <v>1657</v>
       </c>
-      <c r="E305" s="2"/>
-    </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A306" s="2" t="s">
+      <c r="E305" s="6"/>
+    </row>
+    <row r="306" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A306" s="6" t="s">
         <v>1661</v>
       </c>
-      <c r="B306" s="2" t="s">
+      <c r="B306" s="6" t="s">
         <v>1660</v>
       </c>
-      <c r="C306" s="2"/>
-      <c r="D306" s="2" t="s">
+      <c r="C306" s="6"/>
+      <c r="D306" s="6" t="s">
         <v>1662</v>
       </c>
-      <c r="E306" s="2"/>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A307" s="2" t="s">
+      <c r="E306" s="6"/>
+    </row>
+    <row r="307" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="6" t="s">
         <v>1666</v>
       </c>
-      <c r="B307" s="2" t="s">
+      <c r="B307" s="6" t="s">
         <v>1665</v>
       </c>
-      <c r="C307" s="2"/>
-      <c r="D307" s="2" t="s">
+      <c r="C307" s="6"/>
+      <c r="D307" s="6" t="s">
         <v>1667</v>
       </c>
-      <c r="E307" s="2"/>
-    </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A308" s="2" t="s">
+      <c r="E307" s="6"/>
+    </row>
+    <row r="308" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="6" t="s">
         <v>1671</v>
       </c>
-      <c r="B308" s="2" t="s">
+      <c r="B308" s="6" t="s">
         <v>1670</v>
       </c>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2" t="s">
+      <c r="C308" s="6"/>
+      <c r="D308" s="6" t="s">
         <v>1672</v>
       </c>
-      <c r="E308" s="2"/>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A309" s="2" t="s">
+      <c r="E308" s="6"/>
+    </row>
+    <row r="309" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="6" t="s">
         <v>1676</v>
       </c>
-      <c r="B309" s="2" t="s">
+      <c r="B309" s="6" t="s">
         <v>1675</v>
       </c>
-      <c r="C309" s="2"/>
-      <c r="D309" s="2" t="s">
+      <c r="C309" s="6"/>
+      <c r="D309" s="6" t="s">
         <v>1677</v>
       </c>
-      <c r="E309" s="2"/>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A310" s="2" t="s">
+      <c r="E309" s="6"/>
+    </row>
+    <row r="310" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="6" t="s">
         <v>1681</v>
       </c>
-      <c r="B310" s="2" t="s">
+      <c r="B310" s="6" t="s">
         <v>1680</v>
       </c>
-      <c r="C310" s="2"/>
-      <c r="D310" s="2" t="s">
+      <c r="C310" s="6"/>
+      <c r="D310" s="6" t="s">
         <v>1682</v>
       </c>
-      <c r="E310" s="2"/>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A311" s="2" t="s">
+      <c r="E310" s="6"/>
+    </row>
+    <row r="311" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="6" t="s">
         <v>1686</v>
       </c>
-      <c r="B311" s="2" t="s">
+      <c r="B311" s="6" t="s">
         <v>1685</v>
       </c>
-      <c r="C311" s="2"/>
-      <c r="D311" s="2" t="s">
+      <c r="C311" s="6"/>
+      <c r="D311" s="6" t="s">
         <v>1687</v>
       </c>
-      <c r="E311" s="2"/>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A312" s="2" t="s">
+      <c r="E311" s="6"/>
+    </row>
+    <row r="312" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A312" s="6" t="s">
         <v>1691</v>
       </c>
-      <c r="B312" s="2" t="s">
+      <c r="B312" s="6" t="s">
         <v>1690</v>
       </c>
-      <c r="C312" s="2"/>
-      <c r="D312" s="2" t="s">
+      <c r="C312" s="6"/>
+      <c r="D312" s="6" t="s">
         <v>1692</v>
       </c>
-      <c r="E312" s="2"/>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A313" s="2" t="s">
+      <c r="E312" s="6"/>
+    </row>
+    <row r="313" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A313" s="6" t="s">
         <v>1696</v>
       </c>
-      <c r="B313" s="2" t="s">
+      <c r="B313" s="6" t="s">
         <v>1695</v>
       </c>
-      <c r="C313" s="2"/>
-      <c r="D313" s="2" t="s">
+      <c r="C313" s="6"/>
+      <c r="D313" s="6" t="s">
         <v>1697</v>
       </c>
-      <c r="E313" s="2"/>
-    </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A314" s="2" t="s">
+      <c r="E313" s="6"/>
+    </row>
+    <row r="314" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A314" s="6" t="s">
         <v>1701</v>
       </c>
-      <c r="B314" s="2" t="s">
+      <c r="B314" s="6" t="s">
         <v>1700</v>
       </c>
-      <c r="C314" s="2"/>
-      <c r="D314" s="2" t="s">
+      <c r="C314" s="6"/>
+      <c r="D314" s="6" t="s">
         <v>1702</v>
       </c>
-      <c r="E314" s="2"/>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A315" s="2" t="s">
+      <c r="E314" s="6"/>
+    </row>
+    <row r="315" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A315" s="6" t="s">
         <v>1706</v>
       </c>
-      <c r="B315" s="2" t="s">
+      <c r="B315" s="6" t="s">
         <v>1705</v>
       </c>
-      <c r="C315" s="2"/>
-      <c r="D315" s="2" t="s">
+      <c r="C315" s="6"/>
+      <c r="D315" s="6" t="s">
         <v>1707</v>
       </c>
-      <c r="E315" s="2"/>
-    </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A316" s="2" t="s">
+      <c r="E315" s="6"/>
+    </row>
+    <row r="316" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="6" t="s">
         <v>1711</v>
       </c>
-      <c r="B316" s="2" t="s">
+      <c r="B316" s="6" t="s">
         <v>1710</v>
       </c>
-      <c r="C316" s="2"/>
-      <c r="D316" s="2" t="s">
+      <c r="C316" s="6"/>
+      <c r="D316" s="6" t="s">
         <v>1712</v>
       </c>
-      <c r="E316" s="2"/>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A317" s="2" t="s">
+      <c r="E316" s="6"/>
+    </row>
+    <row r="317" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A317" s="6" t="s">
         <v>1716</v>
       </c>
-      <c r="B317" s="2" t="s">
+      <c r="B317" s="6" t="s">
         <v>1715</v>
       </c>
-      <c r="C317" s="2"/>
-      <c r="D317" s="2" t="s">
+      <c r="C317" s="6"/>
+      <c r="D317" s="6" t="s">
         <v>1717</v>
       </c>
-      <c r="E317" s="2"/>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A318" s="2" t="s">
+      <c r="E317" s="6"/>
+    </row>
+    <row r="318" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A318" s="6" t="s">
         <v>1721</v>
       </c>
-      <c r="B318" s="2" t="s">
+      <c r="B318" s="6" t="s">
         <v>1720</v>
       </c>
-      <c r="C318" s="2"/>
-      <c r="D318" s="2" t="s">
+      <c r="C318" s="6"/>
+      <c r="D318" s="6" t="s">
         <v>1722</v>
       </c>
-      <c r="E318" s="2"/>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A319" s="2" t="s">
+      <c r="E318" s="6"/>
+    </row>
+    <row r="319" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A319" s="6" t="s">
         <v>1726</v>
       </c>
-      <c r="B319" s="2" t="s">
+      <c r="B319" s="6" t="s">
         <v>1725</v>
       </c>
-      <c r="C319" s="2"/>
-      <c r="D319" s="2" t="s">
+      <c r="C319" s="6"/>
+      <c r="D319" s="6" t="s">
         <v>1727</v>
       </c>
-      <c r="E319" s="2"/>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A320" s="2" t="s">
+      <c r="E319" s="6"/>
+    </row>
+    <row r="320" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="6" t="s">
         <v>1731</v>
       </c>
-      <c r="B320" s="2" t="s">
+      <c r="B320" s="6" t="s">
         <v>1730</v>
       </c>
-      <c r="C320" s="2"/>
-      <c r="D320" s="2" t="s">
+      <c r="C320" s="6"/>
+      <c r="D320" s="6" t="s">
         <v>1732</v>
       </c>
-      <c r="E320" s="2"/>
-    </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A321" s="2" t="s">
+      <c r="E320" s="6"/>
+    </row>
+    <row r="321" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A321" s="6" t="s">
         <v>1736</v>
       </c>
-      <c r="B321" s="2" t="s">
+      <c r="B321" s="6" t="s">
         <v>1735</v>
       </c>
-      <c r="C321" s="2"/>
-      <c r="D321" s="2" t="s">
+      <c r="C321" s="6"/>
+      <c r="D321" s="6" t="s">
         <v>1737</v>
       </c>
-      <c r="E321" s="2"/>
-    </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A322" s="2" t="s">
+      <c r="E321" s="6"/>
+    </row>
+    <row r="322" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="6" t="s">
         <v>1741</v>
       </c>
-      <c r="B322" s="2" t="s">
+      <c r="B322" s="6" t="s">
         <v>1740</v>
       </c>
-      <c r="C322" s="2"/>
-      <c r="D322" s="2" t="s">
+      <c r="C322" s="6"/>
+      <c r="D322" s="6" t="s">
         <v>1742</v>
       </c>
-      <c r="E322" s="2"/>
-    </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A323" s="2" t="s">
+      <c r="E322" s="6"/>
+    </row>
+    <row r="323" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="6" t="s">
         <v>1746</v>
       </c>
-      <c r="B323" s="2" t="s">
+      <c r="B323" s="6" t="s">
         <v>1745</v>
       </c>
-      <c r="C323" s="2"/>
-      <c r="D323" s="2" t="s">
+      <c r="C323" s="6"/>
+      <c r="D323" s="6" t="s">
         <v>1747</v>
       </c>
-      <c r="E323" s="2"/>
-    </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A324" s="2" t="s">
+      <c r="E323" s="6"/>
+    </row>
+    <row r="324" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="6" t="s">
         <v>1751</v>
       </c>
-      <c r="B324" s="2" t="s">
+      <c r="B324" s="6" t="s">
         <v>1750</v>
       </c>
-      <c r="C324" s="2"/>
-      <c r="D324" s="2" t="s">
+      <c r="C324" s="6"/>
+      <c r="D324" s="6" t="s">
         <v>1752</v>
       </c>
-      <c r="E324" s="2"/>
-    </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A325" s="2" t="s">
+      <c r="E324" s="6"/>
+    </row>
+    <row r="325" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A325" s="6" t="s">
         <v>1756</v>
       </c>
-      <c r="B325" s="2" t="s">
+      <c r="B325" s="6" t="s">
         <v>1755</v>
       </c>
-      <c r="C325" s="2"/>
-      <c r="D325" s="2" t="s">
+      <c r="C325" s="6"/>
+      <c r="D325" s="6" t="s">
         <v>1757</v>
       </c>
-      <c r="E325" s="2"/>
-    </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A326" s="2" t="s">
+      <c r="E325" s="6"/>
+    </row>
+    <row r="326" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A326" s="6" t="s">
         <v>1761</v>
       </c>
-      <c r="B326" s="2" t="s">
+      <c r="B326" s="6" t="s">
         <v>1760</v>
       </c>
-      <c r="C326" s="2"/>
-      <c r="D326" s="2" t="s">
+      <c r="C326" s="6"/>
+      <c r="D326" s="6" t="s">
         <v>1762</v>
       </c>
-      <c r="E326" s="2"/>
-    </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A327" s="2" t="s">
+      <c r="E326" s="6"/>
+    </row>
+    <row r="327" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="6" t="s">
         <v>1766</v>
       </c>
-      <c r="B327" s="2" t="s">
+      <c r="B327" s="6" t="s">
         <v>1765</v>
       </c>
-      <c r="C327" s="2"/>
-      <c r="D327" s="2" t="s">
+      <c r="C327" s="6"/>
+      <c r="D327" s="6" t="s">
         <v>1767</v>
       </c>
-      <c r="E327" s="2"/>
-    </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A328" s="2" t="s">
+      <c r="E327" s="6"/>
+    </row>
+    <row r="328" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="6" t="s">
         <v>1771</v>
       </c>
-      <c r="B328" s="2" t="s">
+      <c r="B328" s="6" t="s">
         <v>1770</v>
       </c>
-      <c r="C328" s="2"/>
-      <c r="D328" s="2" t="s">
+      <c r="C328" s="6"/>
+      <c r="D328" s="6" t="s">
         <v>1772</v>
       </c>
-      <c r="E328" s="2"/>
-    </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A329" s="2" t="s">
+      <c r="E328" s="6"/>
+    </row>
+    <row r="329" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="6" t="s">
         <v>1776</v>
       </c>
-      <c r="B329" s="2" t="s">
+      <c r="B329" s="6" t="s">
         <v>1775</v>
       </c>
-      <c r="C329" s="2"/>
-      <c r="D329" s="2" t="s">
+      <c r="C329" s="6"/>
+      <c r="D329" s="6" t="s">
         <v>1777</v>
       </c>
-      <c r="E329" s="2"/>
-    </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A330" s="2" t="s">
+      <c r="E329" s="6"/>
+    </row>
+    <row r="330" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="6" t="s">
         <v>1781</v>
       </c>
-      <c r="B330" s="2" t="s">
+      <c r="B330" s="6" t="s">
         <v>1780</v>
       </c>
-      <c r="C330" s="2"/>
-      <c r="D330" s="2" t="s">
+      <c r="C330" s="6"/>
+      <c r="D330" s="6" t="s">
         <v>1782</v>
       </c>
-      <c r="E330" s="2"/>
-    </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A331" s="2" t="s">
+      <c r="E330" s="6"/>
+    </row>
+    <row r="331" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="6" t="s">
         <v>1786</v>
       </c>
-      <c r="B331" s="2" t="s">
+      <c r="B331" s="6" t="s">
         <v>1785</v>
       </c>
-      <c r="C331" s="2"/>
-      <c r="D331" s="2" t="s">
+      <c r="C331" s="6"/>
+      <c r="D331" s="6" t="s">
         <v>1787</v>
       </c>
-      <c r="E331" s="2"/>
-    </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A332" s="2" t="s">
+      <c r="E331" s="6"/>
+    </row>
+    <row r="332" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A332" s="6" t="s">
         <v>1791</v>
       </c>
-      <c r="B332" s="2" t="s">
+      <c r="B332" s="6" t="s">
         <v>1790</v>
       </c>
-      <c r="C332" s="2"/>
-      <c r="D332" s="2" t="s">
+      <c r="C332" s="6"/>
+      <c r="D332" s="6" t="s">
         <v>1792</v>
       </c>
-      <c r="E332" s="2"/>
-    </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A333" s="2" t="s">
+      <c r="E332" s="6"/>
+    </row>
+    <row r="333" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A333" s="6" t="s">
         <v>1796</v>
       </c>
-      <c r="B333" s="2" t="s">
+      <c r="B333" s="6" t="s">
         <v>1795</v>
       </c>
-      <c r="C333" s="2"/>
-      <c r="D333" s="2" t="s">
+      <c r="C333" s="6"/>
+      <c r="D333" s="6" t="s">
         <v>1797</v>
       </c>
-      <c r="E333" s="2"/>
-    </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A334" s="2" t="s">
+      <c r="E333" s="6"/>
+    </row>
+    <row r="334" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A334" s="6" t="s">
         <v>1801</v>
       </c>
-      <c r="B334" s="2" t="s">
+      <c r="B334" s="6" t="s">
         <v>1800</v>
       </c>
-      <c r="C334" s="2"/>
-      <c r="D334" s="2" t="s">
+      <c r="C334" s="6"/>
+      <c r="D334" s="6" t="s">
         <v>1802</v>
       </c>
-      <c r="E334" s="2"/>
-    </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A335" s="2" t="s">
+      <c r="E334" s="6"/>
+    </row>
+    <row r="335" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A335" s="6" t="s">
         <v>1806</v>
       </c>
-      <c r="B335" s="2" t="s">
+      <c r="B335" s="6" t="s">
         <v>1805</v>
       </c>
-      <c r="C335" s="2"/>
-      <c r="D335" s="2" t="s">
+      <c r="C335" s="6"/>
+      <c r="D335" s="6" t="s">
         <v>1807</v>
       </c>
-      <c r="E335" s="2"/>
-    </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A336" s="2" t="s">
+      <c r="E335" s="6"/>
+    </row>
+    <row r="336" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="6" t="s">
         <v>1811</v>
       </c>
-      <c r="B336" s="2" t="s">
+      <c r="B336" s="6" t="s">
         <v>1810</v>
       </c>
-      <c r="C336" s="2"/>
-      <c r="D336" s="2" t="s">
+      <c r="C336" s="6"/>
+      <c r="D336" s="6" t="s">
         <v>1812</v>
       </c>
-      <c r="E336" s="2"/>
-    </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A337" s="2" t="s">
+      <c r="E336" s="6"/>
+    </row>
+    <row r="337" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A337" s="6" t="s">
         <v>1816</v>
       </c>
-      <c r="B337" s="2" t="s">
+      <c r="B337" s="6" t="s">
         <v>1815</v>
       </c>
-      <c r="C337" s="2"/>
-      <c r="D337" s="2" t="s">
+      <c r="C337" s="6"/>
+      <c r="D337" s="6" t="s">
         <v>1817</v>
       </c>
-      <c r="E337" s="2"/>
-    </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A338" s="2" t="s">
+      <c r="E337" s="6"/>
+    </row>
+    <row r="338" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A338" s="6" t="s">
         <v>1821</v>
       </c>
-      <c r="B338" s="2" t="s">
+      <c r="B338" s="6" t="s">
         <v>1820</v>
       </c>
-      <c r="C338" s="2"/>
-      <c r="D338" s="2" t="s">
+      <c r="C338" s="6"/>
+      <c r="D338" s="6" t="s">
         <v>1822</v>
       </c>
-      <c r="E338" s="2"/>
-    </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A339" s="2" t="s">
+      <c r="E338" s="6"/>
+    </row>
+    <row r="339" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A339" s="6" t="s">
         <v>1826</v>
       </c>
-      <c r="B339" s="2" t="s">
+      <c r="B339" s="6" t="s">
         <v>1825</v>
       </c>
-      <c r="C339" s="2"/>
-      <c r="D339" s="2" t="s">
+      <c r="C339" s="6"/>
+      <c r="D339" s="6" t="s">
         <v>1827</v>
       </c>
-      <c r="E339" s="2"/>
-    </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A340" s="2" t="s">
+      <c r="E339" s="6"/>
+    </row>
+    <row r="340" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A340" s="6" t="s">
         <v>1831</v>
       </c>
-      <c r="B340" s="2" t="s">
+      <c r="B340" s="6" t="s">
         <v>1830</v>
       </c>
-      <c r="C340" s="2"/>
-      <c r="D340" s="2" t="s">
+      <c r="C340" s="6"/>
+      <c r="D340" s="6" t="s">
         <v>1832</v>
       </c>
-      <c r="E340" s="2"/>
-    </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A341" s="2" t="s">
+      <c r="E340" s="6"/>
+    </row>
+    <row r="341" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A341" s="6" t="s">
         <v>1836</v>
       </c>
-      <c r="B341" s="2" t="s">
+      <c r="B341" s="6" t="s">
         <v>1835</v>
       </c>
-      <c r="C341" s="2"/>
-      <c r="D341" s="2" t="s">
+      <c r="C341" s="6"/>
+      <c r="D341" s="6" t="s">
         <v>1837</v>
       </c>
-      <c r="E341" s="2"/>
-    </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A342" s="2" t="s">
+      <c r="E341" s="6"/>
+    </row>
+    <row r="342" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A342" s="6" t="s">
         <v>1841</v>
       </c>
-      <c r="B342" s="2" t="s">
+      <c r="B342" s="6" t="s">
         <v>1840</v>
       </c>
-      <c r="C342" s="2"/>
-      <c r="D342" s="2" t="s">
+      <c r="C342" s="6"/>
+      <c r="D342" s="6" t="s">
         <v>1842</v>
       </c>
-      <c r="E342" s="2"/>
-    </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A343" s="2" t="s">
+      <c r="E342" s="6"/>
+    </row>
+    <row r="343" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A343" s="6" t="s">
         <v>1846</v>
       </c>
-      <c r="B343" s="2" t="s">
+      <c r="B343" s="6" t="s">
         <v>1845</v>
       </c>
-      <c r="C343" s="2"/>
-      <c r="D343" s="2" t="s">
+      <c r="C343" s="6"/>
+      <c r="D343" s="6" t="s">
         <v>1847</v>
       </c>
-      <c r="E343" s="2"/>
-    </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A344" s="2" t="s">
+      <c r="E343" s="6"/>
+    </row>
+    <row r="344" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A344" s="6" t="s">
         <v>1851</v>
       </c>
-      <c r="B344" s="2" t="s">
+      <c r="B344" s="6" t="s">
         <v>1850</v>
       </c>
-      <c r="C344" s="2"/>
-      <c r="D344" s="2" t="s">
+      <c r="C344" s="6"/>
+      <c r="D344" s="6" t="s">
         <v>1852</v>
       </c>
-      <c r="E344" s="2"/>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A345" s="2" t="s">
+      <c r="E344" s="6"/>
+    </row>
+    <row r="345" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A345" s="6" t="s">
         <v>1856</v>
       </c>
-      <c r="B345" s="2" t="s">
+      <c r="B345" s="6" t="s">
         <v>1855</v>
       </c>
-      <c r="C345" s="2"/>
-      <c r="D345" s="2" t="s">
+      <c r="C345" s="6"/>
+      <c r="D345" s="6" t="s">
         <v>1857</v>
       </c>
-      <c r="E345" s="2"/>
-    </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A346" s="2" t="s">
+      <c r="E345" s="6"/>
+    </row>
+    <row r="346" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A346" s="6" t="s">
         <v>1861</v>
       </c>
-      <c r="B346" s="2" t="s">
+      <c r="B346" s="6" t="s">
         <v>1860</v>
       </c>
-      <c r="C346" s="2"/>
-      <c r="D346" s="2" t="s">
+      <c r="C346" s="6"/>
+      <c r="D346" s="6" t="s">
         <v>1862</v>
       </c>
-      <c r="E346" s="2"/>
-    </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A347" s="2" t="s">
+      <c r="E346" s="6"/>
+    </row>
+    <row r="347" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A347" s="6" t="s">
         <v>1866</v>
       </c>
-      <c r="B347" s="2" t="s">
+      <c r="B347" s="6" t="s">
         <v>1865</v>
       </c>
-      <c r="C347" s="2"/>
-      <c r="D347" s="2" t="s">
+      <c r="C347" s="6"/>
+      <c r="D347" s="6" t="s">
         <v>1867</v>
       </c>
-      <c r="E347" s="2"/>
-    </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A348" s="2" t="s">
+      <c r="E347" s="6"/>
+    </row>
+    <row r="348" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A348" s="6" t="s">
         <v>1871</v>
       </c>
-      <c r="B348" s="2" t="s">
+      <c r="B348" s="6" t="s">
         <v>1870</v>
       </c>
-      <c r="C348" s="2"/>
-      <c r="D348" s="2" t="s">
+      <c r="C348" s="6"/>
+      <c r="D348" s="6" t="s">
         <v>1872</v>
       </c>
-      <c r="E348" s="2"/>
-    </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A349" s="2" t="s">
+      <c r="E348" s="6"/>
+    </row>
+    <row r="349" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A349" s="6" t="s">
         <v>1876</v>
       </c>
-      <c r="B349" s="2" t="s">
+      <c r="B349" s="6" t="s">
         <v>1875</v>
       </c>
-      <c r="C349" s="2"/>
-      <c r="D349" s="2" t="s">
+      <c r="C349" s="6"/>
+      <c r="D349" s="6" t="s">
         <v>1877</v>
       </c>
-      <c r="E349" s="2"/>
-    </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A350" s="2" t="s">
+      <c r="E349" s="6"/>
+    </row>
+    <row r="350" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="6" t="s">
         <v>1881</v>
       </c>
-      <c r="B350" s="2" t="s">
+      <c r="B350" s="6" t="s">
         <v>1880</v>
       </c>
-      <c r="C350" s="2"/>
-      <c r="D350" s="2" t="s">
+      <c r="C350" s="6"/>
+      <c r="D350" s="6" t="s">
         <v>1882</v>
       </c>
-      <c r="E350" s="2"/>
-    </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A351" s="2" t="s">
+      <c r="E350" s="6"/>
+    </row>
+    <row r="351" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A351" s="6" t="s">
         <v>1886</v>
       </c>
-      <c r="B351" s="2" t="s">
+      <c r="B351" s="6" t="s">
         <v>1885</v>
       </c>
-      <c r="C351" s="2"/>
-      <c r="D351" s="2" t="s">
+      <c r="C351" s="6"/>
+      <c r="D351" s="6" t="s">
         <v>1887</v>
       </c>
-      <c r="E351" s="2"/>
-    </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A352" s="2" t="s">
+      <c r="E351" s="6"/>
+    </row>
+    <row r="352" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="6" t="s">
         <v>1891</v>
       </c>
-      <c r="B352" s="2" t="s">
+      <c r="B352" s="6" t="s">
         <v>1890</v>
       </c>
-      <c r="C352" s="2"/>
-      <c r="D352" s="2" t="s">
+      <c r="C352" s="6"/>
+      <c r="D352" s="6" t="s">
         <v>1892</v>
       </c>
-      <c r="E352" s="2"/>
-    </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A353" s="2" t="s">
+      <c r="E352" s="6"/>
+    </row>
+    <row r="353" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A353" s="6" t="s">
         <v>1896</v>
       </c>
-      <c r="B353" s="2" t="s">
+      <c r="B353" s="6" t="s">
         <v>1895</v>
       </c>
-      <c r="C353" s="2"/>
-      <c r="D353" s="2" t="s">
+      <c r="C353" s="6"/>
+      <c r="D353" s="6" t="s">
         <v>1897</v>
       </c>
-      <c r="E353" s="2"/>
-    </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A354" s="2" t="s">
+      <c r="E353" s="6"/>
+    </row>
+    <row r="354" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="6" t="s">
         <v>1901</v>
       </c>
-      <c r="B354" s="2" t="s">
+      <c r="B354" s="6" t="s">
         <v>1900</v>
       </c>
-      <c r="C354" s="2"/>
-      <c r="D354" s="2" t="s">
+      <c r="C354" s="6"/>
+      <c r="D354" s="6" t="s">
         <v>1902</v>
       </c>
-      <c r="E354" s="2"/>
-    </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A355" s="2" t="s">
+      <c r="E354" s="6"/>
+    </row>
+    <row r="355" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A355" s="6" t="s">
         <v>1906</v>
       </c>
-      <c r="B355" s="2" t="s">
+      <c r="B355" s="6" t="s">
         <v>1905</v>
       </c>
-      <c r="C355" s="2"/>
-      <c r="D355" s="2" t="s">
+      <c r="C355" s="6"/>
+      <c r="D355" s="6" t="s">
         <v>1907</v>
       </c>
-      <c r="E355" s="2"/>
-    </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A356" s="2" t="s">
+      <c r="E355" s="6"/>
+    </row>
+    <row r="356" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="6" t="s">
         <v>1911</v>
       </c>
-      <c r="B356" s="2" t="s">
+      <c r="B356" s="6" t="s">
         <v>1910</v>
       </c>
-      <c r="C356" s="2"/>
-      <c r="D356" s="2" t="s">
+      <c r="C356" s="6"/>
+      <c r="D356" s="6" t="s">
         <v>1912</v>
       </c>
-      <c r="E356" s="2"/>
-    </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A357" s="2" t="s">
+      <c r="E356" s="6"/>
+    </row>
+    <row r="357" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A357" s="6" t="s">
         <v>1916</v>
       </c>
-      <c r="B357" s="2" t="s">
+      <c r="B357" s="6" t="s">
         <v>1915</v>
       </c>
-      <c r="C357" s="2"/>
-      <c r="D357" s="2" t="s">
+      <c r="C357" s="6"/>
+      <c r="D357" s="6" t="s">
         <v>1917</v>
       </c>
-      <c r="E357" s="2"/>
-    </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A358" s="2" t="s">
+      <c r="E357" s="6"/>
+    </row>
+    <row r="358" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A358" s="6" t="s">
         <v>1921</v>
       </c>
-      <c r="B358" s="2" t="s">
+      <c r="B358" s="6" t="s">
         <v>1920</v>
       </c>
-      <c r="C358" s="2"/>
-      <c r="D358" s="2" t="s">
+      <c r="C358" s="6"/>
+      <c r="D358" s="6" t="s">
         <v>1922</v>
       </c>
-      <c r="E358" s="2"/>
-    </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A359" s="2" t="s">
+      <c r="E358" s="6"/>
+    </row>
+    <row r="359" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="6" t="s">
         <v>1926</v>
       </c>
-      <c r="B359" s="2" t="s">
+      <c r="B359" s="6" t="s">
         <v>1925</v>
       </c>
-      <c r="C359" s="2"/>
-      <c r="D359" s="2" t="s">
+      <c r="C359" s="6"/>
+      <c r="D359" s="6" t="s">
         <v>1927</v>
       </c>
-      <c r="E359" s="2"/>
-    </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A360" s="2" t="s">
+      <c r="E359" s="6"/>
+    </row>
+    <row r="360" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A360" s="6" t="s">
         <v>1931</v>
       </c>
-      <c r="B360" s="2" t="s">
+      <c r="B360" s="6" t="s">
         <v>1930</v>
       </c>
-      <c r="C360" s="2"/>
-      <c r="D360" s="2" t="s">
+      <c r="C360" s="6"/>
+      <c r="D360" s="6" t="s">
         <v>1932</v>
       </c>
-      <c r="E360" s="2"/>
-    </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A361" s="2" t="s">
+      <c r="E360" s="6"/>
+    </row>
+    <row r="361" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="6" t="s">
         <v>1936</v>
       </c>
-      <c r="B361" s="2" t="s">
+      <c r="B361" s="6" t="s">
         <v>1935</v>
       </c>
-      <c r="C361" s="2"/>
-      <c r="D361" s="2" t="s">
+      <c r="C361" s="6"/>
+      <c r="D361" s="6" t="s">
         <v>1937</v>
       </c>
-      <c r="E361" s="2"/>
-    </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A362" s="2" t="s">
+      <c r="E361" s="6"/>
+    </row>
+    <row r="362" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="6" t="s">
         <v>1941</v>
       </c>
-      <c r="B362" s="2" t="s">
+      <c r="B362" s="6" t="s">
         <v>1940</v>
       </c>
-      <c r="C362" s="2"/>
-      <c r="D362" s="2" t="s">
+      <c r="C362" s="6"/>
+      <c r="D362" s="6" t="s">
         <v>1942</v>
       </c>
-      <c r="E362" s="2"/>
-    </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A363" s="2" t="s">
+      <c r="E362" s="6"/>
+    </row>
+    <row r="363" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="6" t="s">
         <v>1946</v>
       </c>
-      <c r="B363" s="2" t="s">
+      <c r="B363" s="6" t="s">
         <v>1945</v>
       </c>
-      <c r="C363" s="2"/>
-      <c r="D363" s="2" t="s">
+      <c r="C363" s="6"/>
+      <c r="D363" s="6" t="s">
         <v>1947</v>
       </c>
-      <c r="E363" s="2"/>
-    </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A364" s="2" t="s">
+      <c r="E363" s="6"/>
+    </row>
+    <row r="364" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="6" t="s">
         <v>1951</v>
       </c>
-      <c r="B364" s="2" t="s">
+      <c r="B364" s="6" t="s">
         <v>1950</v>
       </c>
-      <c r="C364" s="2"/>
-      <c r="D364" s="2" t="s">
+      <c r="C364" s="6"/>
+      <c r="D364" s="6" t="s">
         <v>1952</v>
       </c>
-      <c r="E364" s="2"/>
-    </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A365" s="2" t="s">
+      <c r="E364" s="6"/>
+    </row>
+    <row r="365" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="6" t="s">
         <v>1956</v>
       </c>
-      <c r="B365" s="2" t="s">
+      <c r="B365" s="6" t="s">
         <v>1955</v>
       </c>
-      <c r="C365" s="2"/>
-      <c r="D365" s="2" t="s">
+      <c r="C365" s="6"/>
+      <c r="D365" s="6" t="s">
         <v>1957</v>
       </c>
-      <c r="E365" s="2"/>
-    </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A366" s="2" t="s">
+      <c r="E365" s="6"/>
+    </row>
+    <row r="366" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="6" t="s">
         <v>1961</v>
       </c>
-      <c r="B366" s="2" t="s">
+      <c r="B366" s="6" t="s">
         <v>1960</v>
       </c>
-      <c r="C366" s="2"/>
-      <c r="D366" s="2" t="s">
+      <c r="C366" s="6"/>
+      <c r="D366" s="6" t="s">
         <v>1962</v>
       </c>
-      <c r="E366" s="2"/>
+      <c r="E366" s="6"/>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A367" s="2" t="s">
@@ -38394,19 +38394,6 @@
         <v>2572</v>
       </c>
       <c r="E487" s="2"/>
-    </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A488" s="2" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B488" s="2" t="s">
-        <v>2606</v>
-      </c>
-      <c r="C488" s="2"/>
-      <c r="D488" s="2" t="s">
-        <v>2607</v>
-      </c>
-      <c r="E488" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>